<commit_message>
Fix OXLDataLink date bug
</commit_message>
<xml_diff>
--- a/tests/data/test_save.xlsx
+++ b/tests/data/test_save.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Ohana\CodingCentre\Efc\pefc\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{529FE602-8C5B-45B6-8FF0-6634E9D8F91C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F0420C0-5A06-4DF2-9A3F-52739B21B8B3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,15 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2153,7 +2161,7 @@
       </c>
       <c r="G7" s="10">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2219,11 +2227,11 @@
       </c>
       <c r="I13" s="6">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
       <c r="J13" s="6">
         <f ca="1">I13-D13</f>
-        <v>1373.0500694444418</v>
+        <v>1517.0500694444418</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2252,7 +2260,7 @@
       </c>
       <c r="I15" s="6">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2315,7 +2323,7 @@
       </c>
       <c r="I18" s="6">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2378,7 +2386,7 @@
       </c>
       <c r="I22" s="6">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2441,7 +2449,7 @@
       </c>
       <c r="I26" s="6">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2507,7 +2515,7 @@
       </c>
       <c r="I30" s="6">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,7 +2685,7 @@
       </c>
       <c r="I39" s="69">
         <f ca="1">TODAY()</f>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -2748,7 +2756,7 @@
       </c>
       <c r="I43" s="77">
         <f t="shared" ca="1" si="0"/>
-        <v>43280</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>